<commit_message>
Add Naumenko and Berdnichenko to list
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Книга Олександр</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Сухоносенко Ілля</t>
+  </si>
+  <si>
+    <t>Ростислав Бердниченко</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Науменко Артем</t>
+  </si>
+  <si>
+    <t>Writing documentation</t>
   </si>
 </sst>
 </file>
@@ -450,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,9 +499,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add hyperlink in MainTasks.xlsx
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -30,23 +30,31 @@
     <t>Андрій Гончарук</t>
   </si>
   <si>
-    <t>Manage the money</t>
-  </si>
-  <si>
     <t>Meetings</t>
   </si>
   <si>
     <t>Сухоносенко Ілля</t>
+  </si>
+  <si>
+    <t>Manage money</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,10 +167,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -170,8 +179,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,7 +464,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,15 +487,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -492,7 +503,10 @@
       <c r="B5" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add hyperlink to manage the money
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -55,10 +55,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,10 +179,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -182,8 +191,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +476,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +506,7 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -516,7 +527,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolving merge conflict by rename hyperlink
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -30,9 +30,6 @@
     <t>Андрій Гончарук</t>
   </si>
   <si>
-    <t>Manage the money</t>
-  </si>
-  <si>
     <t>Meetings</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Writing documentation</t>
+  </si>
+  <si>
+    <t>Manage money</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,31 +499,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add hyperlink to monitor project progress
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24666F09-D727-48EA-8BCD-914076BE349D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,12 +187,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -472,11 +473,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,47 +491,48 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8CFCC163-078F-475E-837A-B38904A21522}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add hyperlink to Folder "Monitor project progress"
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5EDCBE-FF08-4936-8E75-F0207C227891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,12 +187,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -472,11 +473,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,47 +491,48 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9B4A1BB5-1B0D-4C6D-85D6-6DEB88DE832F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'master' into manage-the-money"
This reverts commit bdf59209900387c683bb0e6d42383512a7dc5219, reversing
changes made to 6c976e42c6405ad5f5b36d32109c6f6632febfa1.
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24666F09-D727-48EA-8BCD-914076BE349D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,12 +186,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -473,11 +472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,48 +490,47 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{8CFCC163-078F-475E-837A-B38904A21522}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add hyper-link to your folder
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5EDCBE-FF08-4936-8E75-F0207C227891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CE5EDCBE-FF08-4936-8E75-F0207C227891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B9F5CAB-D53C-411A-8313-7A6F91447478}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -195,8 +195,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +515,7 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -531,8 +531,9 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{9B4A1BB5-1B0D-4C6D-85D6-6DEB88DE832F}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{5AC0060C-B20B-4ABA-A122-4646574036C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add hyperlink  to Meetings
</commit_message>
<xml_diff>
--- a/MainTasks.xlsx
+++ b/MainTasks.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CE5EDCBE-FF08-4936-8E75-F0207C227891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B9F5CAB-D53C-411A-8313-7A6F91447478}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E285709-11EA-48A1-BAD3-03A679E823D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -184,19 +184,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,7 +476,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +490,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -499,7 +498,7 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -507,7 +506,7 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -515,15 +514,15 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -532,8 +531,9 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{9B4A1BB5-1B0D-4C6D-85D6-6DEB88DE832F}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{5AC0060C-B20B-4ABA-A122-4646574036C0}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{BD67BAEA-6002-43D4-BAB2-2A48ED4B1EB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>